<commit_message>
Basic implementation of Aufgabe 2 into Project for Aufgabe 3 and rudimentary implementation of Pageflipping as drawing technique to avoid flickering and for a smoother appeareance
</commit_message>
<xml_diff>
--- a/Aufgaben/Aufgabe 2/Cellular Test.xlsx
+++ b/Aufgaben/Aufgabe 2/Cellular Test.xlsx
@@ -24,12 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>3,4,5,7</t>
-  </si>
-  <si>
-    <t>0,1,5</t>
   </si>
   <si>
     <t>0,1,2,3,4,5,7</t>
@@ -106,7 +103,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -120,6 +117,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -403,7 +402,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,18 +415,18 @@
         <v>0</v>
       </c>
       <c r="C1" s="1">
-        <v>1.4</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25">
@@ -482,9 +481,21 @@
     </row>
     <row r="8" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="5"/>
+    </row>
     <row r="13" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>